<commit_message>
update templates; add quickview tab
</commit_message>
<xml_diff>
--- a/www/templates/additional_standard_terms.xlsx
+++ b/www/templates/additional_standard_terms.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vchung/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09DFB3F5-0AC3-0E4E-A4C8-2BC074330ED1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66F50AEA-91D9-A049-BE79-EA73F1EC6CDB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12060" yWindow="460" windowWidth="16740" windowHeight="15840" xr2:uid="{31BA8282-D0C2-47F7-B15B-5ECFEECDB2D3}"/>
+    <workbookView xWindow="1860" yWindow="460" windowWidth="26940" windowHeight="15840" xr2:uid="{31BA8282-D0C2-47F7-B15B-5ECFEECDB2D3}"/>
   </bookViews>
   <sheets>
     <sheet name="new_terms" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
   <si>
     <t>inputDataType</t>
   </si>
@@ -92,6 +92,24 @@
   </si>
   <si>
     <t>outputDataType</t>
+  </si>
+  <si>
+    <t>ontologySource</t>
+  </si>
+  <si>
+    <t>ontologyID</t>
+  </si>
+  <si>
+    <t>ontologyUrl</t>
+  </si>
+  <si>
+    <t>ontology unique ID for term, e.g. C3099</t>
+  </si>
+  <si>
+    <t>ontology source of new term, e.g. NCIT</t>
+  </si>
+  <si>
+    <t>link to ontology term, e.g. https://ncit.nci.nih.gov/ncitbrowser/ConceptReport.jsp?dictionary=NCI_Thesaurus&amp;code=C3099</t>
   </si>
 </sst>
 </file>
@@ -128,11 +146,13 @@
       <sz val="12"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -488,7 +508,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74343AE0-FCE9-4359-9F0E-4B5D07198D62}">
-  <dimension ref="A1:J25"/>
+  <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -498,120 +518,154 @@
   <cols>
     <col min="1" max="1" width="15.83203125" customWidth="1"/>
     <col min="2" max="2" width="28.6640625" customWidth="1"/>
-    <col min="3" max="3" width="35.6640625" customWidth="1"/>
-    <col min="4" max="4" width="20.6640625" customWidth="1"/>
-    <col min="5" max="5" width="19.83203125" customWidth="1"/>
-    <col min="6" max="6" width="9.6640625" customWidth="1"/>
-    <col min="7" max="7" width="14.6640625" customWidth="1"/>
-    <col min="8" max="8" width="22.6640625" customWidth="1"/>
-    <col min="9" max="9" width="13.1640625" customWidth="1"/>
+    <col min="3" max="3" width="20" customWidth="1"/>
+    <col min="4" max="4" width="36.5" customWidth="1"/>
+    <col min="5" max="5" width="40.1640625" customWidth="1"/>
+    <col min="6" max="6" width="19.83203125" customWidth="1"/>
+    <col min="7" max="7" width="9.6640625" customWidth="1"/>
+    <col min="8" max="8" width="14.6640625" customWidth="1"/>
+    <col min="9" max="9" width="22.6640625" customWidth="1"/>
+    <col min="10" max="10" width="13.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B2" s="1"/>
       <c r="C2" s="2"/>
-      <c r="E2" s="1"/>
+      <c r="D2" s="2"/>
       <c r="F2" s="1"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="2"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="3"/>
       <c r="I2" s="2"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J2" s="2"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C3" s="2"/>
-      <c r="H3" s="2"/>
+      <c r="D3" s="2"/>
       <c r="I3" s="2"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J3" s="2"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C4" s="6"/>
-      <c r="G4" s="3"/>
-      <c r="J4" s="3"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="D4" s="6"/>
+      <c r="H4" s="3"/>
+      <c r="K4" s="3"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C5" s="6"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="D5" s="6"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C6" s="6"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="D6" s="6"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
       <c r="D7" s="8"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E7" s="8"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B8" s="8"/>
       <c r="C8" s="7"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="8"/>
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
       <c r="H8" s="7"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="I8" s="7"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B9" s="8"/>
       <c r="C9" s="7"/>
-      <c r="D9" s="8"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="D9" s="7"/>
+      <c r="E9" s="8"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B10" s="8"/>
       <c r="C10" s="9"/>
-      <c r="D10" s="8"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="D10" s="9"/>
+      <c r="E10" s="8"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B11" s="5"/>
       <c r="C11" s="7"/>
-      <c r="D11" s="8"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="D11" s="7"/>
+      <c r="E11" s="8"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C12" s="6"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="D12" s="6"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B13" s="3"/>
       <c r="C13" s="9"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="D13" s="9"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B14" s="3"/>
       <c r="C14" s="9"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="D14" s="9"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C15" s="6"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="D15" s="6"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C16" s="6"/>
-    </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="D16" s="6"/>
+    </row>
+    <row r="17" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C17" s="6"/>
-    </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="D17" s="6"/>
+    </row>
+    <row r="18" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C18" s="6"/>
-    </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="D18" s="6"/>
+    </row>
+    <row r="19" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C19" s="6"/>
-    </row>
-    <row r="20" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="D19" s="6"/>
+    </row>
+    <row r="20" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C20" s="6"/>
-    </row>
-    <row r="21" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="D20" s="6"/>
+    </row>
+    <row r="21" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C21" s="6"/>
-    </row>
-    <row r="22" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="D21" s="6"/>
+    </row>
+    <row r="22" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C22" s="6"/>
-    </row>
-    <row r="23" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="D22" s="6"/>
+    </row>
+    <row r="23" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C23" s="6"/>
-    </row>
-    <row r="24" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="D23" s="6"/>
+    </row>
+    <row r="24" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C24" s="6"/>
-    </row>
-    <row r="25" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="D24" s="6"/>
+    </row>
+    <row r="25" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -633,7 +687,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91FADD7E-9694-A74E-93B9-75899B8A9F3C}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -665,6 +719,30 @@
       </c>
       <c r="B3" s="1" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -759,18 +837,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -920,18 +998,18 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E421B32D-69A3-450A-8E2A-BBC4266B7A20}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0C92A347-FC36-478F-955F-48E5A3590BDF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E421B32D-69A3-450A-8E2A-BBC4266B7A20}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>